<commit_message>
better handles bad URLs
</commit_message>
<xml_diff>
--- a/tests/data/071_demo.xlsx
+++ b/tests/data/071_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/kurrawong/VocExcel/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AC750D-4E4E-7949-BDC8-B7839FB2C3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815238AE-B789-8346-A3E4-4CFD2168244E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44920" yWindow="580" windowWidth="54100" windowHeight="28040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1562,9 +1562,6 @@
     <t>Silky@en, Chinese silk chicken@en, jedwabisty@pl</t>
   </si>
   <si>
-    <t>http://example.com/chicken-breeds/sultan</t>
-  </si>
-  <si>
     <t>Sultan</t>
   </si>
   <si>
@@ -1578,6 +1575,9 @@
   </si>
   <si>
     <t>Definition taken directly from Wikipedia</t>
+  </si>
+  <si>
+    <t>http://example.com/chicken-breeds/this is a %%bad__-*&amp;URI</t>
   </si>
 </sst>
 </file>
@@ -2030,6 +2030,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2044,9 +2047,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3938,12 +3938,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:4" s="36" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -3963,7 +3963,7 @@
       <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="61" t="s">
         <v>179</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -7162,7 +7162,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0.15"/>
@@ -7179,16 +7179,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
@@ -7256,25 +7256,25 @@
         <v>188</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:8" ht="152" x14ac:dyDescent="0.15">
       <c r="A5" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="G5" s="20" t="s">
         <v>192</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -7573,16 +7573,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -7711,13 +7711,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
@@ -9099,11 +9099,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="25" t="s">
@@ -9204,11 +9204,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">

</xml_diff>